<commit_message>
removed the google sheets link from the code so that people wont vandalize it lmao
</commit_message>
<xml_diff>
--- a/maps_and_descriptors.xlsx
+++ b/maps_and_descriptors.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="782">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="783">
   <si>
     <t>1a</t>
   </si>
@@ -1172,6 +1172,9 @@
   </si>
   <si>
     <t>October</t>
+  </si>
+  <si>
+    <t>summit up-side</t>
   </si>
   <si>
     <t>Old Site Remix (A-Side)</t>
@@ -4597,129 +4600,132 @@
       </c>
     </row>
     <row r="140">
+      <c r="B140" s="1" t="s">
+        <v>387</v>
+      </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="7" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="141">
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="7" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="142">
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="7" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="143">
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="7" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
     </row>
     <row r="144">
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="7" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="145">
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
       <c r="F145" s="7" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
     </row>
     <row r="146">
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
       <c r="F146" s="7" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="147">
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
       <c r="F147" s="7" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
     </row>
     <row r="148">
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
       <c r="F148" s="7" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
     </row>
     <row r="149">
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
       <c r="F149" s="7" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="150">
       <c r="D150" s="1"/>
       <c r="E150" s="1"/>
       <c r="F150" s="7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="151">
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
       <c r="F151" s="7" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
     </row>
     <row r="152">
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
       <c r="F152" s="7" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
     </row>
     <row r="153">
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
       <c r="F153" s="7" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="154">
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
       <c r="F154" s="7" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="155">
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
       <c r="F155" s="7" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="156">
       <c r="D156" s="1"/>
       <c r="E156" s="1"/>
       <c r="F156" s="7" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="157">
       <c r="D157" s="1"/>
       <c r="E157" s="1"/>
       <c r="F157" s="7" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
     </row>
     <row r="158">
@@ -4731,1538 +4737,1538 @@
       <c r="D159" s="1"/>
       <c r="E159" s="1"/>
       <c r="F159" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="160">
       <c r="D160" s="1"/>
       <c r="E160" s="1"/>
       <c r="F160" s="7" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
     </row>
     <row r="161">
       <c r="D161" s="1"/>
       <c r="E161" s="1"/>
       <c r="F161" s="7" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="162">
       <c r="D162" s="1"/>
       <c r="E162" s="1"/>
       <c r="F162" s="7" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
     </row>
     <row r="163">
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
       <c r="F163" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
     </row>
     <row r="164">
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
       <c r="F164" s="7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="165">
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
       <c r="F165" s="7" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
     </row>
     <row r="166">
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
       <c r="F166" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
     </row>
     <row r="167">
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
       <c r="F167" s="7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="168">
       <c r="F168" s="7" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
     </row>
     <row r="169">
       <c r="F169" s="7" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
     </row>
     <row r="170">
       <c r="F170" s="7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
     </row>
     <row r="171">
       <c r="F171" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="172">
       <c r="F172" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
     </row>
     <row r="173">
       <c r="F173" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="174">
       <c r="F174" s="7" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
     </row>
     <row r="175">
       <c r="F175" s="7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="176">
       <c r="F176" s="7" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="177">
       <c r="F177" s="13" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="178">
       <c r="F178" s="14" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="179">
       <c r="F179" s="14" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="180">
       <c r="F180" s="14" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="181">
       <c r="F181" s="14" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="182">
       <c r="F182" s="14" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="183">
       <c r="F183" s="14" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="184">
       <c r="F184" s="14" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="185">
       <c r="F185" s="14" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="186">
       <c r="F186" s="14" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="187">
       <c r="F187" s="14" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="188">
       <c r="F188" s="14" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="189">
       <c r="F189" s="14" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="190">
       <c r="F190" s="14" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="191">
       <c r="F191" s="14" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="192">
       <c r="F192" s="14" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="193">
       <c r="F193" s="14" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="194">
       <c r="F194" s="14" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="195">
       <c r="F195" s="14" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="196">
       <c r="F196" s="14" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="197">
       <c r="F197" s="14" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="198">
       <c r="F198" s="14" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="199">
       <c r="F199" s="14" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="200">
       <c r="F200" s="14" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="201">
       <c r="F201" s="14" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="202">
       <c r="F202" s="14" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="203">
       <c r="F203" s="14" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="204">
       <c r="F204" s="14" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="205">
       <c r="F205" s="14" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="206">
       <c r="F206" s="14" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="207">
       <c r="F207" s="14" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="208">
       <c r="F208" s="14" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
     </row>
     <row r="209">
       <c r="F209" s="14" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="210">
       <c r="F210" s="14" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
     </row>
     <row r="211">
       <c r="F211" s="14" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="212">
       <c r="F212" s="14" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="213">
       <c r="F213" s="14" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="214">
       <c r="F214" s="14" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="215">
       <c r="F215" s="14" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
     </row>
     <row r="216">
       <c r="F216" s="14" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="217">
       <c r="F217" s="14" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
     </row>
     <row r="218">
       <c r="F218" s="14" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="219">
       <c r="F219" s="14" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="220">
       <c r="F220" s="14" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
     </row>
     <row r="221">
       <c r="F221" s="14" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="222">
       <c r="F222" s="14" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
     </row>
     <row r="223">
       <c r="F223" s="14" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="224">
       <c r="F224" s="14" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="225">
       <c r="F225" s="14" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
     </row>
     <row r="226">
       <c r="F226" s="14" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
     </row>
     <row r="227">
       <c r="F227" s="14" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
     </row>
     <row r="228">
       <c r="F228" s="14" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="229">
       <c r="F229" s="14" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
     </row>
     <row r="230">
       <c r="F230" s="14" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="231">
       <c r="F231" s="14" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="232">
       <c r="F232" s="14" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="233">
       <c r="F233" s="14" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="234">
       <c r="F234" s="14" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="235">
       <c r="F235" s="14" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="236">
       <c r="F236" s="14" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="237">
       <c r="F237" s="14" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="238">
       <c r="F238" s="14" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="239">
       <c r="F239" s="14" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="240">
       <c r="F240" s="14" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="241">
       <c r="F241" s="14" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="242">
       <c r="F242" s="14" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="243">
       <c r="F243" s="14" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="244">
       <c r="F244" s="14" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="245">
       <c r="F245" s="14" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="246">
       <c r="F246" s="14" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="247">
       <c r="F247" s="14" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="248">
       <c r="F248" s="14" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="249">
       <c r="F249" s="14" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="250">
       <c r="F250" s="14" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="251">
       <c r="F251" s="14" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
     </row>
     <row r="252">
       <c r="F252" s="14" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="253">
       <c r="F253" s="14" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
     </row>
     <row r="254">
       <c r="F254" s="14" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="255">
       <c r="F255" s="14" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
     </row>
     <row r="256">
       <c r="F256" s="14" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="257">
       <c r="F257" s="14" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="258">
       <c r="F258" s="14" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
     </row>
     <row r="259">
       <c r="F259" s="14" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="260">
       <c r="F260" s="14" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
     </row>
     <row r="261">
       <c r="F261" s="14" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="262">
       <c r="F262" s="14" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
     </row>
     <row r="263">
       <c r="F263" s="14" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="264">
       <c r="F264" s="14" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
     </row>
     <row r="265">
       <c r="F265" s="14" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
     </row>
     <row r="266">
       <c r="F266" s="14" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="267">
       <c r="F267" s="14" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="268">
       <c r="F268" s="14" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="269">
       <c r="F269" s="14" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="270">
       <c r="F270" s="14" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="271">
       <c r="F271" s="14" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="272">
       <c r="F272" s="14" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="273">
       <c r="F273" s="14" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
     </row>
     <row r="274">
       <c r="F274" s="14" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="275">
       <c r="F275" s="14" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
     </row>
     <row r="276">
       <c r="F276" s="14" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="277">
       <c r="F277" s="14" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
     </row>
     <row r="278">
       <c r="F278" s="14" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
     </row>
     <row r="279">
       <c r="F279" s="14" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
     </row>
     <row r="280">
       <c r="F280" s="14" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="281">
       <c r="F281" s="14" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="282">
       <c r="F282" s="14" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
     </row>
     <row r="283">
       <c r="F283" s="14" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="284">
       <c r="F284" s="14" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="285">
       <c r="F285" s="14" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
     <row r="286">
       <c r="F286" s="14" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="287">
       <c r="F287" s="14" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="288">
       <c r="F288" s="14" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="289">
       <c r="F289" s="14" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
     </row>
     <row r="290">
       <c r="F290" s="14" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="291">
       <c r="F291" s="14" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="292">
       <c r="F292" s="14" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="293">
       <c r="F293" s="14" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="294">
       <c r="F294" s="14" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
     </row>
     <row r="295">
       <c r="F295" s="14" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="296">
       <c r="F296" s="14" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
     </row>
     <row r="297">
       <c r="F297" s="14" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="298">
       <c r="F298" s="14" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="299">
       <c r="F299" s="14" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
     </row>
     <row r="300">
       <c r="F300" s="14" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="301">
       <c r="F301" s="14" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
     </row>
     <row r="302">
       <c r="F302" s="14" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="303">
       <c r="F303" s="14" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="304">
       <c r="F304" s="14" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="305">
       <c r="F305" s="14" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
     </row>
     <row r="306">
       <c r="F306" s="14" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
     </row>
     <row r="307">
       <c r="F307" s="14" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="308">
       <c r="F308" s="14" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="309">
       <c r="F309" s="14" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="310">
       <c r="F310" s="14" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="311">
       <c r="F311" s="14" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="312">
       <c r="F312" s="14" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
     </row>
     <row r="313">
       <c r="F313" s="14" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
     </row>
     <row r="314">
       <c r="F314" s="14" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="315">
       <c r="F315" s="14" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="316">
       <c r="F316" s="14" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="317">
       <c r="F317" s="14" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="318">
       <c r="F318" s="14" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="319">
       <c r="F319" s="14" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="320">
       <c r="F320" s="14" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="321">
       <c r="F321" s="14" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="322">
       <c r="F322" s="14" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="323">
       <c r="F323" s="15" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="324">
       <c r="F324" s="16" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
     </row>
     <row r="325">
       <c r="F325" s="16" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
     </row>
     <row r="326">
       <c r="F326" s="16" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="327">
       <c r="F327" s="16" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="328">
       <c r="F328" s="16" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="329">
       <c r="F329" s="16" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="330">
       <c r="F330" s="16" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
     </row>
     <row r="331">
       <c r="F331" s="16" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
     </row>
     <row r="332">
       <c r="F332" s="16" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="333">
       <c r="F333" s="16" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="334">
       <c r="F334" s="16" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="335">
       <c r="F335" s="16" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
     </row>
     <row r="336">
       <c r="F336" s="16" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="337">
       <c r="F337" s="16" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
     </row>
     <row r="338">
       <c r="F338" s="16" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="339">
       <c r="F339" s="16" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="340">
       <c r="F340" s="16" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="341">
       <c r="F341" s="16" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="342">
       <c r="F342" s="16" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="343">
       <c r="F343" s="16" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="344">
       <c r="F344" s="16" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="345">
       <c r="F345" s="16" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="346">
       <c r="F346" s="16" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
     </row>
     <row r="347">
       <c r="F347" s="16" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="348">
       <c r="F348" s="16" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
     </row>
     <row r="349">
       <c r="F349" s="16" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
     </row>
     <row r="350">
       <c r="F350" s="16" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="351">
       <c r="F351" s="16" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="352">
       <c r="F352" s="16" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="353">
       <c r="F353" s="16" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="354">
       <c r="F354" s="16" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="355">
       <c r="F355" s="16" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
     </row>
     <row r="356">
       <c r="F356" s="16" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="357">
       <c r="F357" s="16" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="358">
       <c r="F358" s="16" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
     </row>
     <row r="359">
       <c r="F359" s="16" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="360">
       <c r="F360" s="16" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="361">
       <c r="F361" s="16" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="362">
       <c r="F362" s="16" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="363">
       <c r="F363" s="16" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="364">
       <c r="F364" s="16" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="365">
       <c r="F365" s="16" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="366">
       <c r="F366" s="16" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="367">
       <c r="F367" s="16" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="368">
       <c r="F368" s="16" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="369">
       <c r="F369" s="16" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="370">
       <c r="F370" s="16" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="371">
       <c r="F371" s="16" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="372">
       <c r="F372" s="16" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="373">
       <c r="F373" s="16" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="374">
       <c r="F374" s="16" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="375">
       <c r="F375" s="16" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="376">
       <c r="F376" s="16" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="377">
       <c r="F377" s="16" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="378">
       <c r="F378" s="16" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="379">
       <c r="F379" s="16" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="380">
       <c r="F380" s="16" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="381">
       <c r="F381" s="16" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="382">
       <c r="F382" s="16" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
     <row r="383">
       <c r="F383" s="16" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="384">
       <c r="F384" s="16" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="385">
       <c r="F385" s="16" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="386">
       <c r="F386" s="16" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="387">
       <c r="F387" s="16" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="388">
       <c r="F388" s="16" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="389">
       <c r="F389" s="16" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="390">
       <c r="F390" s="16" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="391">
       <c r="F391" s="16" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="392">
       <c r="F392" s="16" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="393">
       <c r="F393" s="16" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
     </row>
     <row r="394">
       <c r="F394" s="16" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="395">
       <c r="F395" s="16" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="396">
       <c r="F396" s="16" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="397">
       <c r="F397" s="16" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="398">
       <c r="F398" s="16" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
     </row>
     <row r="399">
       <c r="F399" s="16" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="400">
       <c r="F400" s="16" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="401">
       <c r="F401" s="16" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
     </row>
     <row r="402">
       <c r="F402" s="16" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="403">
       <c r="F403" s="16" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="404">
       <c r="F404" s="16" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="405">
       <c r="F405" s="16" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="406">
       <c r="F406" s="16" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="407">
       <c r="F407" s="16" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="408">
       <c r="F408" s="16" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="409">
       <c r="F409" s="16" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="410">
       <c r="F410" s="16" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="411">
       <c r="F411" s="16" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="412">
       <c r="F412" s="16" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="413">
       <c r="F413" s="16" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
     </row>
     <row r="414">
       <c r="F414" s="16" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="415">
       <c r="F415" s="16" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="416">
       <c r="F416" s="16" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="417">
       <c r="F417" s="16" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
     </row>
     <row r="418">
       <c r="F418" s="16" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="419">
       <c r="F419" s="16" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="420">
       <c r="F420" s="16" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="421">
       <c r="F421" s="16" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="422">
       <c r="F422" s="16" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
     </row>
     <row r="423">
       <c r="F423" s="16" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
     </row>
     <row r="424">
       <c r="F424" s="16" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="425">
       <c r="F425" s="16" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
     </row>
     <row r="426">
       <c r="F426" s="16" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="427">
       <c r="F427" s="16" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="428">
       <c r="F428" s="16" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="429">
       <c r="F429" s="16" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="430">
       <c r="F430" s="16" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="431">
       <c r="F431" s="16" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="432">
       <c r="F432" s="16" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="433">
       <c r="F433" s="16" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="434">
       <c r="F434" s="16" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="435">
       <c r="F435" s="16" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
     </row>
     <row r="436">
       <c r="F436" s="16" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="437">
       <c r="F437" s="16" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
     </row>
     <row r="438">
       <c r="F438" s="16" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="439">
       <c r="F439" s="16" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="440">
       <c r="F440" s="16" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="441">
       <c r="F441" s="16" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
     </row>
     <row r="442">
       <c r="F442" s="16" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
     </row>
     <row r="443">
       <c r="F443" s="16" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
     </row>
     <row r="444">
       <c r="F444" s="16" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="445">
       <c r="F445" s="16" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="446">
       <c r="F446" s="16" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="447">
       <c r="F447" s="16" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="448">
       <c r="F448" s="16" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="449">
       <c r="F449" s="16" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="450">
       <c r="F450" s="16" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="451">
       <c r="F451" s="16" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="452">
       <c r="F452" s="16" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="453">
       <c r="F453" s="16" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="454">
       <c r="F454" s="16" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="455">
       <c r="F455" s="16" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="456">
       <c r="F456" s="16" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="457">
       <c r="F457" s="16" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="458">
       <c r="F458" s="16" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
     </row>
     <row r="459">
       <c r="F459" s="16" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
     </row>
     <row r="460">
       <c r="F460" s="17" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="461">
       <c r="F461" s="18" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
     </row>
     <row r="462">
       <c r="F462" s="18" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="463">
@@ -6272,367 +6278,367 @@
     </row>
     <row r="464">
       <c r="F464" s="18" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
     </row>
     <row r="465">
       <c r="F465" s="18" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
     </row>
     <row r="466">
       <c r="F466" s="18" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="467">
       <c r="F467" s="18" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="468">
       <c r="F468" s="18" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
     <row r="469">
       <c r="F469" s="18" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
     </row>
     <row r="470">
       <c r="F470" s="18" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="471">
       <c r="F471" s="18" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
     </row>
     <row r="472">
       <c r="F472" s="18" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
     </row>
     <row r="473">
       <c r="F473" s="18" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
     </row>
     <row r="474">
       <c r="F474" s="18" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
     </row>
     <row r="475">
       <c r="F475" s="18" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="476">
       <c r="F476" s="18" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
     </row>
     <row r="477">
       <c r="F477" s="18" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
     </row>
     <row r="478">
       <c r="F478" s="18" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
     </row>
     <row r="479">
       <c r="F479" s="18" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
     </row>
     <row r="480">
       <c r="F480" s="18" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="481">
       <c r="F481" s="18" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
     </row>
     <row r="482">
       <c r="F482" s="18" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
     </row>
     <row r="483">
       <c r="F483" s="18" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
     </row>
     <row r="484">
       <c r="F484" s="18" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
     </row>
     <row r="485">
       <c r="F485" s="18" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
     </row>
     <row r="486">
       <c r="F486" s="18" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
     </row>
     <row r="487">
       <c r="F487" s="18" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
     </row>
     <row r="488">
       <c r="F488" s="18" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
     </row>
     <row r="489">
       <c r="F489" s="18" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="490">
       <c r="F490" s="18" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
     </row>
     <row r="491">
       <c r="F491" s="18" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
     </row>
     <row r="492">
       <c r="F492" s="18" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
     </row>
     <row r="493">
       <c r="F493" s="18" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
     </row>
     <row r="494">
       <c r="F494" s="18" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
     </row>
     <row r="495">
       <c r="F495" s="18" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
     </row>
     <row r="496">
       <c r="F496" s="18" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
     </row>
     <row r="497">
       <c r="F497" s="18" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="498">
       <c r="F498" s="18" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
     </row>
     <row r="499">
       <c r="F499" s="18" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
     </row>
     <row r="500">
       <c r="F500" s="18" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="501">
       <c r="F501" s="18" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
     </row>
     <row r="502">
       <c r="F502" s="18" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
     </row>
     <row r="503">
       <c r="F503" s="18" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
     </row>
     <row r="504">
       <c r="F504" s="18" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
     </row>
     <row r="505">
       <c r="F505" s="18" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
     </row>
     <row r="506">
       <c r="F506" s="18" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
     </row>
     <row r="507">
       <c r="F507" s="18" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
     </row>
     <row r="508">
       <c r="F508" s="18" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
     </row>
     <row r="509">
       <c r="F509" s="18" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
     </row>
     <row r="510">
       <c r="F510" s="18" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
     </row>
     <row r="511">
       <c r="F511" s="18" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
     </row>
     <row r="512">
       <c r="F512" s="18" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
     </row>
     <row r="513">
       <c r="F513" s="18" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
     </row>
     <row r="514">
       <c r="F514" s="18" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
     </row>
     <row r="515">
       <c r="F515" s="18" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
     </row>
     <row r="516">
       <c r="F516" s="18" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
     </row>
     <row r="517">
       <c r="F517" s="18" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
     </row>
     <row r="518">
       <c r="F518" s="18" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
     </row>
     <row r="519">
       <c r="F519" s="18" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
     </row>
     <row r="520">
       <c r="F520" s="18" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
     </row>
     <row r="521">
       <c r="F521" s="18" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
     </row>
     <row r="522">
       <c r="F522" s="18" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
     </row>
     <row r="523">
       <c r="F523" s="18" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
     </row>
     <row r="524">
       <c r="F524" s="18" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
     </row>
     <row r="525">
       <c r="F525" s="18" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
     </row>
     <row r="526">
       <c r="F526" s="18" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
     </row>
     <row r="527">
       <c r="F527" s="18" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
     </row>
     <row r="528">
       <c r="F528" s="18" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
     </row>
     <row r="529">
       <c r="F529" s="18" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
     </row>
     <row r="530">
       <c r="F530" s="18" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
     </row>
     <row r="531">
       <c r="F531" s="18" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
     </row>
     <row r="532">
       <c r="F532" s="18" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="533">
       <c r="F533" s="18" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
     </row>
     <row r="534">
       <c r="F534" s="18" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="535">
       <c r="F535" s="18" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
     </row>
     <row r="536">
       <c r="F536" s="18" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="537">

</xml_diff>